<commit_message>
Update Product selection file
</commit_message>
<xml_diff>
--- a/storage/app/excel/export-templates/product-selection.xlsx
+++ b/storage/app/excel/export-templates/product-selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\home\erp-evolet\storage\app\excel\export-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CAF97D-2BF7-4E79-AADA-D73589E5E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC61B82-68C0-4428-801A-1F755D7EC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2A26C44-2D1F-413C-A575-90AC71DB4886}"/>
   </bookViews>
@@ -548,36 +548,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,6 +561,36 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{C8660A90-0DA4-4A06-87EC-B3A80C258B0F}"/>
@@ -926,7 +926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -938,9 +938,9 @@
     <col min="5" max="5" width="9.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="52" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="52" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="42" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="42" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="42" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.28515625" style="5" customWidth="1"/>
@@ -967,27 +967,27 @@
       <c r="E1" s="1"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="48"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
       <c r="AA1" s="4" t="s">
         <v>1</v>
       </c>
@@ -996,21 +996,21 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
-      <c r="AG1" s="39" t="s">
+      <c r="AG1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="42" t="s">
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="AK1" s="43"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="45" t="s">
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="49"/>
+      <c r="AM1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="47"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="52"/>
     </row>
     <row r="2" spans="1:41" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1034,13 +1034,13 @@
       <c r="G2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="39" t="s">
         <v>49</v>
       </c>
       <c r="K2" s="9" t="s">
@@ -1145,9 +1145,9 @@
       <c r="E3" s="18"/>
       <c r="F3" s="20"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="50"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="21"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -1188,9 +1188,9 @@
       <c r="E4" s="18"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
       <c r="K4" s="26"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>

</xml_diff>

<commit_message>
Add forecast columns separately for ProductSelection export
</commit_message>
<xml_diff>
--- a/storage/app/excel/export-templates/product-selection.xlsx
+++ b/storage/app/excel/export-templates/product-selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\home\erp-evolet\storage\app\excel\export-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC61B82-68C0-4428-801A-1F755D7EC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE66798-0F46-47CD-8E97-89F5D15E58DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2A26C44-2D1F-413C-A575-90AC71DB4886}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>REGISTERING COUNTRIES</t>
   </si>
@@ -42,9 +42,6 @@
     <t>YES/NO</t>
   </si>
   <si>
-    <t>FORECAST ESTIMATES</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -88,15 +85,6 @@
   </si>
   <si>
     <t>DOSSIER TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YEAR 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YEAR 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YEAR 3</t>
   </si>
   <si>
     <t>Note: Please provide required info for highlighted cells.</t>
@@ -375,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -398,50 +386,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,15 +428,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -508,12 +450,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,33 +498,6 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -924,9 +833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB251C2F-0DEB-447E-982C-891A3EAD04FA}">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -934,13 +843,13 @@
     <col min="1" max="1" width="5.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="84.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="22" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="42" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="42" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="42" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="37" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="37" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.28515625" style="5" customWidth="1"/>
@@ -967,27 +876,27 @@
       <c r="E1" s="1"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
       <c r="AA1" s="4" t="s">
         <v>1</v>
       </c>
@@ -996,380 +905,353 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
-      <c r="AG1" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="52"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+      <c r="AK1"/>
+      <c r="AL1"/>
+      <c r="AM1"/>
+      <c r="AN1"/>
+      <c r="AO1"/>
     </row>
     <row r="2" spans="1:41" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="G2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="Y2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="24"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="39" t="s">
+      <c r="B10" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="10" t="s">
+      <c r="B20" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="12" t="s">
+      <c r="B23" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AM2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AN2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO2" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="29"/>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="37" t="s">
+      <c r="B24" s="32" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:AO3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="L1:Z1"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AJ1:AL1"/>
-    <mergeCell ref="AM1:AO1"/>
   </mergeCells>
   <conditionalFormatting sqref="L1:Z1048576">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="between">

</xml_diff>